<commit_message>
added margin of victory
</commit_message>
<xml_diff>
--- a/fullStats.xlsx
+++ b/fullStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexfick/Documents/School/Second year/math50/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0B873AD8-2CC2-1343-A127-F1A5489EB834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AF56AA90-D303-5E40-8FEE-BFA5779BA266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="16940"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="87">
   <si>
     <t>Team</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>Successes</t>
+  </si>
+  <si>
+    <t>MOV</t>
   </si>
 </sst>
 </file>
@@ -1139,15 +1142,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB1000"/>
+  <dimension ref="A1:AC1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="Y155" sqref="Y155"/>
+    <sheetView tabSelected="1" topLeftCell="R103" workbookViewId="0">
+      <selection activeCell="AC122" sqref="AC122:AC151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1232,8 +1235,11 @@
       <c r="AB1" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1318,8 +1324,11 @@
       <c r="AB2" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC2" s="1">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1404,8 +1413,11 @@
       <c r="AB3" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC3" s="1">
+        <v>7.28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1490,8 +1502,11 @@
       <c r="AB4" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC4" s="1">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1576,8 +1591,11 @@
       <c r="AB5" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC5" s="1">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -1662,8 +1680,11 @@
       <c r="AB6" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC6" s="1">
+        <v>-0.39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -1748,8 +1769,11 @@
       <c r="AB7" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC7" s="1">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -1834,8 +1858,11 @@
       <c r="AB8" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC8" s="1">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -1920,8 +1947,11 @@
       <c r="AB9" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC9" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -2006,8 +2036,11 @@
       <c r="AB10" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC10" s="1">
+        <v>-7.72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -2092,8 +2125,11 @@
       <c r="AB11" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC11" s="1">
+        <v>5.54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -2178,8 +2214,11 @@
       <c r="AB12" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC12" s="1">
+        <v>-8.48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -2264,8 +2303,11 @@
       <c r="AB13" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC13" s="1">
+        <v>-3.48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -2350,8 +2392,11 @@
       <c r="AB14" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC14" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -2436,8 +2481,11 @@
       <c r="AB15" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC15" s="1">
+        <v>-3.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -2522,8 +2570,11 @@
       <c r="AB16" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC16" s="1">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -2608,8 +2659,11 @@
       <c r="AB17" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC17" s="1">
+        <v>4.45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -2694,8 +2748,11 @@
       <c r="AB18" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC18" s="1">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -2780,8 +2837,11 @@
       <c r="AB19" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC19" s="1">
+        <v>2.63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -2866,8 +2926,11 @@
       <c r="AB20" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC20" s="1">
+        <v>-0.99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -2952,8 +3015,11 @@
       <c r="AB21" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC21" s="1">
+        <v>-0.12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -3038,8 +3104,11 @@
       <c r="AB22" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC22" s="1">
+        <v>-8.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -3124,8 +3193,11 @@
       <c r="AB23" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC23" s="1">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -3210,8 +3282,11 @@
       <c r="AB24" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC24" s="1">
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -3296,8 +3371,11 @@
       <c r="AB25" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC25" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -3382,8 +3460,11 @@
       <c r="AB26" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC26" s="1">
+        <v>-8.8800000000000008</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -3468,8 +3549,11 @@
       <c r="AB27" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC27" s="1">
+        <v>-5.46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -3554,8 +3638,11 @@
       <c r="AB28" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC28" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -3640,8 +3727,11 @@
       <c r="AB29" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC29" s="1">
+        <v>2.29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -3726,8 +3816,11 @@
       <c r="AB30" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC30" s="1">
+        <v>6.04</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -3812,8 +3905,11 @@
       <c r="AB31" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC31" s="1">
+        <v>-3.38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -3898,8 +3994,11 @@
       <c r="AB32" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC32" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -3984,8 +4083,11 @@
       <c r="AB33" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC33" s="1">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -4070,8 +4172,11 @@
       <c r="AB34" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC34" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -4156,8 +4261,11 @@
       <c r="AB35" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC35" s="1">
+        <v>-1.93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -4242,8 +4350,11 @@
       <c r="AB36" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC36" s="1">
+        <v>-0.89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -4328,8 +4439,11 @@
       <c r="AB37" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC37" s="1">
+        <v>-8.44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>66</v>
       </c>
@@ -4414,8 +4528,11 @@
       <c r="AB38" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC38" s="1">
+        <v>2.2599999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>58</v>
       </c>
@@ -4500,8 +4617,11 @@
       <c r="AB39" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC39" s="1">
+        <v>4.93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -4586,8 +4706,11 @@
       <c r="AB40" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC40" s="1">
+        <v>-4.47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>67</v>
       </c>
@@ -4672,8 +4795,11 @@
       <c r="AB41" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC41" s="1">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>71</v>
       </c>
@@ -4758,8 +4884,11 @@
       <c r="AB42" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC42" s="1">
+        <v>-7.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -4844,8 +4973,11 @@
       <c r="AB43" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC43" s="1">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>60</v>
       </c>
@@ -4930,8 +5062,11 @@
       <c r="AB44" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC44" s="1">
+        <v>6.18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>68</v>
       </c>
@@ -5016,8 +5151,11 @@
       <c r="AB45" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC45" s="1">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>73</v>
       </c>
@@ -5102,8 +5240,11 @@
       <c r="AB46" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC46" s="1">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -5188,8 +5329,11 @@
       <c r="AB47" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC47" s="1">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -5274,8 +5418,11 @@
       <c r="AB48" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC48" s="1">
+        <v>5.89</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>62</v>
       </c>
@@ -5360,8 +5507,11 @@
       <c r="AB49" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC49" s="1">
+        <v>-5.56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -5446,8 +5596,11 @@
       <c r="AB50" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC50" s="1">
+        <v>-0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>74</v>
       </c>
@@ -5532,8 +5685,11 @@
       <c r="AB51" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC51" s="1">
+        <v>2.31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>75</v>
       </c>
@@ -5618,8 +5774,11 @@
       <c r="AB52" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC52" s="1">
+        <v>-10.64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -5704,8 +5863,11 @@
       <c r="AB53" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC53" s="1">
+        <v>-9.31</v>
+      </c>
+    </row>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -5790,8 +5952,11 @@
       <c r="AB54" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC54" s="1">
+        <v>5.58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>76</v>
       </c>
@@ -5876,8 +6041,11 @@
       <c r="AB55" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC55" s="1">
+        <v>5.82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>50</v>
       </c>
@@ -5962,8 +6130,11 @@
       <c r="AB56" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC56" s="1">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>51</v>
       </c>
@@ -6048,8 +6219,11 @@
       <c r="AB57" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC57" s="1">
+        <v>-3.68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>69</v>
       </c>
@@ -6134,8 +6308,11 @@
       <c r="AB58" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC58" s="1">
+        <v>-1.74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>77</v>
       </c>
@@ -6220,8 +6397,11 @@
       <c r="AB59" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC59" s="1">
+        <v>-0.47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>54</v>
       </c>
@@ -6306,8 +6486,11 @@
       <c r="AB60" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC60" s="1">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>55</v>
       </c>
@@ -6392,8 +6575,11 @@
       <c r="AB61" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC61" s="1">
+        <v>-1.83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>26</v>
       </c>
@@ -6478,8 +6664,11 @@
       <c r="AB62" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC62" s="1">
+        <v>-7.97</v>
+      </c>
+    </row>
+    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>27</v>
       </c>
@@ -6564,8 +6753,11 @@
       <c r="AB63" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC63" s="1">
+        <v>6.31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>56</v>
       </c>
@@ -6650,8 +6842,11 @@
       <c r="AB64" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC64" s="1">
+        <v>-0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="65" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>29</v>
       </c>
@@ -6736,8 +6931,11 @@
       <c r="AB65" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC65" s="1">
+        <v>-6.75</v>
+      </c>
+    </row>
+    <row r="66" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>30</v>
       </c>
@@ -6822,8 +7020,11 @@
       <c r="AB66" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC66" s="1">
+        <v>-3.08</v>
+      </c>
+    </row>
+    <row r="67" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>57</v>
       </c>
@@ -6908,8 +7109,11 @@
       <c r="AB67" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC67" s="1">
+        <v>-7.89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -6994,8 +7198,11 @@
       <c r="AB68" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC68" s="1">
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="69" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>58</v>
       </c>
@@ -7080,8 +7287,11 @@
       <c r="AB69" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC69" s="1">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>34</v>
       </c>
@@ -7166,8 +7376,11 @@
       <c r="AB70" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC70" s="1">
+        <v>-3.56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>67</v>
       </c>
@@ -7252,8 +7465,11 @@
       <c r="AB71" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC71" s="1">
+        <v>-8.7100000000000009</v>
+      </c>
+    </row>
+    <row r="72" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>36</v>
       </c>
@@ -7338,8 +7554,11 @@
       <c r="AB72" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC72" s="1">
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>37</v>
       </c>
@@ -7424,8 +7643,11 @@
       <c r="AB73" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC73" s="1">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>60</v>
       </c>
@@ -7510,8 +7732,11 @@
       <c r="AB74" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC74" s="1">
+        <v>6.44</v>
+      </c>
+    </row>
+    <row r="75" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>68</v>
       </c>
@@ -7596,8 +7821,11 @@
       <c r="AB75" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC75" s="1">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>40</v>
       </c>
@@ -7682,8 +7910,11 @@
       <c r="AB76" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC76" s="1">
+        <v>-1.07</v>
+      </c>
+    </row>
+    <row r="77" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>41</v>
       </c>
@@ -7768,8 +7999,11 @@
       <c r="AB77" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC77" s="1">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>42</v>
       </c>
@@ -7854,8 +8088,11 @@
       <c r="AB78" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC78" s="1">
+        <v>10.08</v>
+      </c>
+    </row>
+    <row r="79" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>62</v>
       </c>
@@ -7940,8 +8177,11 @@
       <c r="AB79" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC79" s="1">
+        <v>-4.3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>63</v>
       </c>
@@ -8026,8 +8266,11 @@
       <c r="AB80" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC80" s="1">
+        <v>-1.29</v>
+      </c>
+    </row>
+    <row r="81" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>45</v>
       </c>
@@ -8112,8 +8355,11 @@
       <c r="AB81" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC81" s="1">
+        <v>-6.45</v>
+      </c>
+    </row>
+    <row r="82" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>46</v>
       </c>
@@ -8198,8 +8444,11 @@
       <c r="AB82" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC82" s="1">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>64</v>
       </c>
@@ -8284,8 +8533,11 @@
       <c r="AB83" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC83" s="1">
+        <v>-1.01</v>
+      </c>
+    </row>
+    <row r="84" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>48</v>
       </c>
@@ -8370,8 +8622,11 @@
       <c r="AB84" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC84" s="1">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="85" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>49</v>
       </c>
@@ -8456,8 +8711,11 @@
       <c r="AB85" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC85" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>50</v>
       </c>
@@ -8542,8 +8800,11 @@
       <c r="AB86" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC86" s="1">
+        <v>-1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>51</v>
       </c>
@@ -8628,8 +8889,11 @@
       <c r="AB87" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC87" s="1">
+        <v>-2.04</v>
+      </c>
+    </row>
+    <row r="88" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>69</v>
       </c>
@@ -8714,8 +8978,11 @@
       <c r="AB88" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC88" s="1">
+        <v>-1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>53</v>
       </c>
@@ -8800,8 +9067,11 @@
       <c r="AB89" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC89" s="1">
+        <v>6.24</v>
+      </c>
+    </row>
+    <row r="90" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>54</v>
       </c>
@@ -8886,8 +9156,11 @@
       <c r="AB90" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC90" s="1">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="91" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>65</v>
       </c>
@@ -8972,8 +9245,11 @@
       <c r="AB91" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC91" s="1">
+        <v>-4.67</v>
+      </c>
+    </row>
+    <row r="92" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>26</v>
       </c>
@@ -9058,8 +9334,11 @@
       <c r="AB92" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC92" s="1">
+        <v>-6.02</v>
+      </c>
+    </row>
+    <row r="93" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>27</v>
       </c>
@@ -9144,8 +9423,11 @@
       <c r="AB93" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC93" s="1">
+        <v>4.4400000000000004</v>
+      </c>
+    </row>
+    <row r="94" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>56</v>
       </c>
@@ -9230,8 +9512,11 @@
       <c r="AB94" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC94" s="1">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>29</v>
       </c>
@@ -9316,8 +9601,11 @@
       <c r="AB95" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC95" s="1">
+        <v>-1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>30</v>
       </c>
@@ -9402,8 +9690,11 @@
       <c r="AB96" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC96" s="1">
+        <v>-8.41</v>
+      </c>
+    </row>
+    <row r="97" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>57</v>
       </c>
@@ -9488,8 +9779,11 @@
       <c r="AB97" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC97" s="1">
+        <v>-9.61</v>
+      </c>
+    </row>
+    <row r="98" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>32</v>
       </c>
@@ -9574,8 +9868,11 @@
       <c r="AB98" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC98" s="1">
+        <v>-1.28</v>
+      </c>
+    </row>
+    <row r="99" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>58</v>
       </c>
@@ -9660,8 +9957,11 @@
       <c r="AB99" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC99" s="1">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="100" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>59</v>
       </c>
@@ -9746,8 +10046,11 @@
       <c r="AB100" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC100" s="1">
+        <v>-0.24</v>
+      </c>
+    </row>
+    <row r="101" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>35</v>
       </c>
@@ -9832,8 +10135,11 @@
       <c r="AB101" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC101" s="1">
+        <v>6.46</v>
+      </c>
+    </row>
+    <row r="102" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>36</v>
       </c>
@@ -9918,8 +10224,11 @@
       <c r="AB102" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC102" s="1">
+        <v>4.7699999999999996</v>
+      </c>
+    </row>
+    <row r="103" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>37</v>
       </c>
@@ -10004,8 +10313,11 @@
       <c r="AB103" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC103" s="1">
+        <v>3.33</v>
+      </c>
+    </row>
+    <row r="104" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>60</v>
       </c>
@@ -10090,8 +10402,11 @@
       <c r="AB104" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC104" s="1">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="105" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>39</v>
       </c>
@@ -10176,8 +10491,11 @@
       <c r="AB105" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC105" s="1">
+        <v>-1.72</v>
+      </c>
+    </row>
+    <row r="106" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>40</v>
       </c>
@@ -10262,8 +10580,11 @@
       <c r="AB106" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC106" s="1">
+        <v>-2.6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>61</v>
       </c>
@@ -10348,8 +10669,11 @@
       <c r="AB107" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC107" s="1">
+        <v>-0.23</v>
+      </c>
+    </row>
+    <row r="108" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>42</v>
       </c>
@@ -10434,8 +10758,11 @@
       <c r="AB108" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC108" s="1">
+        <v>8.8699999999999992</v>
+      </c>
+    </row>
+    <row r="109" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>62</v>
       </c>
@@ -10520,8 +10847,11 @@
       <c r="AB109" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC109" s="1">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>63</v>
       </c>
@@ -10606,8 +10936,11 @@
       <c r="AB110" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC110" s="1">
+        <v>-1.33</v>
+      </c>
+    </row>
+    <row r="111" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>45</v>
       </c>
@@ -10692,8 +11025,11 @@
       <c r="AB111" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC111" s="1">
+        <v>-9.2100000000000009</v>
+      </c>
+    </row>
+    <row r="112" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>46</v>
       </c>
@@ -10778,8 +11114,11 @@
       <c r="AB112" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="113" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC112" s="1">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>64</v>
       </c>
@@ -10864,8 +11203,11 @@
       <c r="AB113" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="114" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC113" s="1">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="114" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>48</v>
       </c>
@@ -10950,8 +11292,11 @@
       <c r="AB114" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="115" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC114" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>49</v>
       </c>
@@ -11036,8 +11381,11 @@
       <c r="AB115" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="116" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC115" s="1">
+        <v>-9.34</v>
+      </c>
+    </row>
+    <row r="116" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>50</v>
       </c>
@@ -11122,8 +11470,11 @@
       <c r="AB116" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="117" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC116" s="1">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>51</v>
       </c>
@@ -11208,8 +11559,11 @@
       <c r="AB117" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="118" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC117" s="1">
+        <v>-1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>52</v>
       </c>
@@ -11294,8 +11648,11 @@
       <c r="AB118" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="119" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC118" s="1">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="119" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>53</v>
       </c>
@@ -11380,8 +11737,11 @@
       <c r="AB119" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="120" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC119" s="1">
+        <v>6.09</v>
+      </c>
+    </row>
+    <row r="120" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>54</v>
       </c>
@@ -11466,8 +11826,11 @@
       <c r="AB120" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="121" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC120" s="1">
+        <v>5.26</v>
+      </c>
+    </row>
+    <row r="121" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>65</v>
       </c>
@@ -11552,8 +11915,11 @@
       <c r="AB121" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="122" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC121" s="1">
+        <v>-2.9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>26</v>
       </c>
@@ -11638,8 +12004,11 @@
       <c r="AB122" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="123" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="AC122" s="1">
+        <v>-5.45</v>
+      </c>
+    </row>
+    <row r="123" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>27</v>
       </c>
@@ -11724,8 +12093,11 @@
       <c r="AB123" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="124" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC123" s="1">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="124" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>28</v>
       </c>
@@ -11810,8 +12182,11 @@
       <c r="AB124" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="125" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC124" s="1">
+        <v>-3.74</v>
+      </c>
+    </row>
+    <row r="125" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>29</v>
       </c>
@@ -11896,8 +12271,11 @@
       <c r="AB125" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="126" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC125" s="1">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="126" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>30</v>
       </c>
@@ -11982,8 +12360,11 @@
       <c r="AB126" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="127" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC126" s="1">
+        <v>-7.04</v>
+      </c>
+    </row>
+    <row r="127" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>31</v>
       </c>
@@ -12068,8 +12449,11 @@
       <c r="AB127" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="128" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC127" s="1">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="128" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>32</v>
       </c>
@@ -12154,8 +12538,11 @@
       <c r="AB128" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="129" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC128" s="1">
+        <v>-3.04</v>
+      </c>
+    </row>
+    <row r="129" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>33</v>
       </c>
@@ -12240,8 +12627,11 @@
       <c r="AB129" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="130" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC129" s="1">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="130" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>34</v>
       </c>
@@ -12326,8 +12716,11 @@
       <c r="AB130" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="131" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC130" s="1">
+        <v>-0.15</v>
+      </c>
+    </row>
+    <row r="131" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>35</v>
       </c>
@@ -12412,8 +12805,11 @@
       <c r="AB131" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="132" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC131" s="1">
+        <v>5.98</v>
+      </c>
+    </row>
+    <row r="132" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>36</v>
       </c>
@@ -12498,8 +12894,11 @@
       <c r="AB132" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="133" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC132" s="1">
+        <v>8.48</v>
+      </c>
+    </row>
+    <row r="133" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>37</v>
       </c>
@@ -12584,8 +12983,11 @@
       <c r="AB133" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="134" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC133" s="1">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="134" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>38</v>
       </c>
@@ -12670,8 +13072,11 @@
       <c r="AB134" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="135" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC134" s="1">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="135" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>39</v>
       </c>
@@ -12756,8 +13161,11 @@
       <c r="AB135" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="136" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC135" s="1">
+        <v>-1.55</v>
+      </c>
+    </row>
+    <row r="136" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>40</v>
       </c>
@@ -12842,8 +13250,11 @@
       <c r="AB136" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="137" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC136" s="1">
+        <v>-6.21</v>
+      </c>
+    </row>
+    <row r="137" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>41</v>
       </c>
@@ -12928,8 +13339,11 @@
       <c r="AB137" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="138" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC137" s="1">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="138" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>42</v>
       </c>
@@ -13014,8 +13428,11 @@
       <c r="AB138" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="139" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC138" s="1">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>43</v>
       </c>
@@ -13100,8 +13517,11 @@
       <c r="AB139" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="140" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC139" s="1">
+        <v>2.23</v>
+      </c>
+    </row>
+    <row r="140" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>44</v>
       </c>
@@ -13186,8 +13606,11 @@
       <c r="AB140" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="141" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC140" s="1">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>45</v>
       </c>
@@ -13272,8 +13695,11 @@
       <c r="AB141" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="142" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC141" s="1">
+        <v>-3.56</v>
+      </c>
+    </row>
+    <row r="142" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>46</v>
       </c>
@@ -13358,8 +13784,11 @@
       <c r="AB142" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="143" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC142" s="1">
+        <v>3.41</v>
+      </c>
+    </row>
+    <row r="143" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>47</v>
       </c>
@@ -13444,8 +13873,11 @@
       <c r="AB143" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="144" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC143" s="1">
+        <v>-4.82</v>
+      </c>
+    </row>
+    <row r="144" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>48</v>
       </c>
@@ -13530,8 +13962,11 @@
       <c r="AB144" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="145" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC144" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>49</v>
       </c>
@@ -13616,8 +14051,11 @@
       <c r="AB145" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="146" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC145" s="1">
+        <v>-9.3699999999999992</v>
+      </c>
+    </row>
+    <row r="146" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>50</v>
       </c>
@@ -13702,8 +14140,11 @@
       <c r="AB146" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="147" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC146" s="1">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>51</v>
       </c>
@@ -13788,8 +14229,11 @@
       <c r="AB147" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="148" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC147" s="1">
+        <v>-6.99</v>
+      </c>
+    </row>
+    <row r="148" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>52</v>
       </c>
@@ -13874,8 +14318,11 @@
       <c r="AB148" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="149" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC148" s="1">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="149" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>53</v>
       </c>
@@ -13960,8 +14407,11 @@
       <c r="AB149" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="150" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC149" s="1">
+        <v>7.78</v>
+      </c>
+    </row>
+    <row r="150" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>54</v>
       </c>
@@ -14046,8 +14496,11 @@
       <c r="AB150" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="151" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC150" s="1">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>55</v>
       </c>
@@ -14132,32 +14585,35 @@
       <c r="AB151" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="152" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC151" s="1">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="152" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AB152" s="3"/>
     </row>
-    <row r="153" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AB153" s="3"/>
     </row>
-    <row r="154" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AB154" s="3"/>
     </row>
-    <row r="155" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AB155" s="3"/>
     </row>
-    <row r="156" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AB156" s="3"/>
     </row>
-    <row r="157" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AB157" s="3"/>
     </row>
-    <row r="158" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AB158" s="3"/>
     </row>
-    <row r="159" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AB159" s="3"/>
     </row>
-    <row r="160" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AB160" s="3"/>
     </row>
     <row r="161" spans="28:28" x14ac:dyDescent="0.2">

</xml_diff>